<commit_message>
WF-97: Info margin laba
</commit_message>
<xml_diff>
--- a/public/public/produk/pengaturan_harga/import_pengaturan_harga.xlsx
+++ b/public/public/produk/pengaturan_harga/import_pengaturan_harga.xlsx
@@ -1,30 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\trading\public\public\produk\pengaturan_harga\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="21000" windowHeight="11415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Data Harga</t>
   </si>
@@ -86,31 +76,46 @@
     <t>Satuan 5</t>
   </si>
   <si>
-    <t>Margin 1</t>
+    <t>Margin Bawah 1</t>
+  </si>
+  <si>
+    <t>Margin Atas 1</t>
   </si>
   <si>
     <t>Harga 1</t>
   </si>
   <si>
-    <t>Margin 2</t>
+    <t>Margin Bawah 2</t>
+  </si>
+  <si>
+    <t>Margin Atas 2</t>
   </si>
   <si>
     <t>Harga 2</t>
   </si>
   <si>
-    <t>Margin 3</t>
+    <t>Margin Bawah 3</t>
+  </si>
+  <si>
+    <t>Margin Atas 3</t>
   </si>
   <si>
     <t>Harga 3</t>
   </si>
   <si>
-    <t>Margin 4</t>
+    <t>Margin Bawah 4</t>
+  </si>
+  <si>
+    <t>Margin Atas 4</t>
   </si>
   <si>
     <t>Harga 4</t>
   </si>
   <si>
-    <t>Margin 5</t>
+    <t>Margin Bawah 5</t>
+  </si>
+  <si>
+    <t>Margin Atas 5</t>
   </si>
   <si>
     <t>Harga 5</t>
@@ -119,13 +124,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,8 +155,159 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +326,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -202,6 +550,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -225,11 +586,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -242,35 +845,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -319,7 +969,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -354,7 +1004,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -528,24 +1178,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" outlineLevelRow="6"/>
+  <cols>
+    <col min="16" max="16" width="16.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="19" max="19" width="16.2857142857143" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
+    <col min="22" max="22" width="16.2857142857143" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="25" max="25" width="16.2857142857143" customWidth="1"/>
+    <col min="26" max="26" width="14" customWidth="1"/>
+    <col min="28" max="28" width="16.2857142857143" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,8 +1231,9 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,8 +1261,9 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:26">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -631,8 +1291,9 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -658,8 +1319,9 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:30">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -687,123 +1349,149 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="8"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="13"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:30">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="Q6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="S6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="T6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="V6" s="10" t="s">
         <v>26</v>
       </c>
       <c r="W6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="X6" s="12" t="s">
         <v>28</v>
       </c>
       <c r="Y6" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="Z6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+    <row r="7" spans="1:30">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="P5:Y5"/>
+    <mergeCell ref="F5:O5"/>
+    <mergeCell ref="P5:AD5"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>